<commit_message>
Additions/Changes by Rohit to Connor's Code
</commit_message>
<xml_diff>
--- a/tools/inf_GUI_materials.xlsx
+++ b/tools/inf_GUI_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith248/Documents/Hyades/Latest_Gui/pyhy/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahari4\Downloads\pyhy\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94300E78-FE81-6E45-8C17-C97FC46B875A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F56CCCA-CDED-4A70-9AD1-BF5C5BAF9676}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="5700" windowWidth="20020" windowHeight="17300" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7572" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Material</t>
   </si>
@@ -551,21 +545,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116FF25-5E59-4448-8946-7353F238B6E9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.796875" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -605,7 +599,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -625,7 +619,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -645,7 +639,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -665,7 +659,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -685,7 +679,7 @@
         <v>1.845</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -705,7 +699,7 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -725,7 +719,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -745,7 +739,7 @@
         <v>7.19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -765,7 +759,7 @@
         <v>8.8550000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -785,7 +779,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -805,7 +799,7 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -825,7 +819,7 @@
         <v>1.1850000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -845,7 +839,7 @@
         <v>7.8719999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -865,7 +859,7 @@
         <v>5.3230000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -878,14 +872,14 @@
       <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="2">
-        <v>0.5</v>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F16" s="2">
         <v>3.58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -905,7 +899,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -925,7 +919,7 @@
         <v>11.14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -945,7 +939,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -965,7 +959,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -985,7 +979,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -1005,7 +999,7 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1025,7 +1019,7 @@
         <v>19.236999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1045,7 +1039,7 @@
         <v>7.1390000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -1066,7 +1060,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F25">
+  <sortState ref="A4:F25">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reorganized some buttons and inputs on the inf_GUI.py. Cleaned up the readme to make it more instructive, deleted some unused files.
</commit_message>
<xml_diff>
--- a/tools/inf_GUI_materials.xlsx
+++ b/tools/inf_GUI_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahari4\Downloads\pyhy\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjkri\PycharmProjects\pyhy\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F56CCCA-CDED-4A70-9AD1-BF5C5BAF9676}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAD610-7806-44FB-921F-98ADDC474BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7572" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,21 +545,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116FF25-5E59-4448-8946-7353F238B6E9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.796875" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.69921875" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,287 +579,287 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>26.981999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2">
+        <v>79</v>
+      </c>
+      <c r="D3" s="2">
+        <v>195.97</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2">
+        <v>997</v>
+      </c>
+      <c r="C5" s="2">
+        <v>83</v>
+      </c>
+      <c r="D5" s="2">
+        <v>208.98</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>481</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2">
+        <v>581</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2">
+        <v>51.996000000000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2">
+        <v>112</v>
+      </c>
+      <c r="C8" s="2">
         <v>29</v>
       </c>
-      <c r="B2" s="2">
+      <c r="D8" s="2">
+        <v>63.545999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>8.8550000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2">
+        <v>341</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12.010999999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2">
+        <v>800</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2">
+        <v>502</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.2406999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5.9134000000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.1850000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2">
+        <v>182</v>
+      </c>
+      <c r="C12" s="2">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>55.85</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7.8719999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2">
+        <v>320</v>
+      </c>
+      <c r="C13" s="2">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2">
+        <v>72.64</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5.3230000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
         <v>1.42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B15" s="2">
         <v>727</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F15" s="2">
         <v>2.64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>26.981999999999999</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="2">
-        <v>51</v>
-      </c>
-      <c r="C5" s="2">
-        <v>79</v>
-      </c>
-      <c r="D5" s="2">
-        <v>195.97</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>19.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2">
-        <v>81</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.845</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2">
-        <v>997</v>
-      </c>
-      <c r="C7" s="2">
-        <v>83</v>
-      </c>
-      <c r="D7" s="2">
-        <v>208.98</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>9.7799999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2">
-        <v>481</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2">
-        <v>40.078000000000003</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="2">
-        <v>581</v>
-      </c>
-      <c r="C9" s="2">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2">
-        <v>51.996000000000002</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>7.19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2">
-        <v>112</v>
-      </c>
-      <c r="C10" s="2">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2">
-        <v>63.545999999999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>8.8550000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2">
-        <v>341</v>
-      </c>
-      <c r="C11" s="2">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2">
-        <v>12.010999999999999</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>3.51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="2">
-        <v>800</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3.32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2">
-        <v>502</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3.2406999999999999</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5.9134000000000002</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.1850000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2">
-        <v>182</v>
-      </c>
-      <c r="C14" s="2">
-        <v>26</v>
-      </c>
-      <c r="D14" s="2">
-        <v>55.85</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <v>7.8719999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="2">
-        <v>320</v>
-      </c>
-      <c r="C15" s="2">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2">
-        <v>72.64</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>5.3230000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -879,7 +879,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -919,7 +919,7 @@
         <v>11.14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -939,7 +939,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -959,7 +959,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -979,7 +979,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -999,7 +999,7 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>19.236999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>7.1390000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -1060,8 +1060,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:F25">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
+    <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed ShockVelocity class to work with new HyadesOutput.x, cleaned up plot.py to work with new ShockVelocity
</commit_message>
<xml_diff>
--- a/tools/inf_GUI_materials.xlsx
+++ b/tools/inf_GUI_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjkri\PycharmProjects\pyhy\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAD610-7806-44FB-921F-98ADDC474BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0CCABF-B676-497B-A1E0-7CFAF35FE5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{788FEA1F-C42A-E042-AAB3-BEEFA7D13A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Material</t>
   </si>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116FF25-5E59-4448-8946-7353F238B6E9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -832,8 +832,8 @@
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2">
-        <v>1</v>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F14" s="2">
         <v>1.42</v>

</xml_diff>